<commit_message>
Calculate Arbitrage Bid / Ask
</commit_message>
<xml_diff>
--- a/Calculate.xlsx
+++ b/Calculate.xlsx
@@ -5,27 +5,36 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Workspaces\GitHub\cctx-Binance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixBrenkel\Source\Workspaces\GitHub\cctx-Binance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD049DE5-F7C3-48C7-93A2-13A2F8D6D868}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6C8D3D-8D00-40D2-951B-34C859967EE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="2580" windowWidth="18600" windowHeight="10260" xr2:uid="{40CD4046-9C5B-4F58-A310-3C08BDEFF96F}"/>
+    <workbookView xWindow="9030" yWindow="3450" windowWidth="22875" windowHeight="15675" xr2:uid="{40CD4046-9C5B-4F58-A310-3C08BDEFF96F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>BTC/USDT</t>
   </si>
@@ -34,12 +43,36 @@
   </si>
   <si>
     <t>ETH/USDT</t>
+  </si>
+  <si>
+    <t>Base Coin</t>
+  </si>
+  <si>
+    <t>USDT</t>
+  </si>
+  <si>
+    <t>BTC</t>
+  </si>
+  <si>
+    <t>Verkaufen</t>
+  </si>
+  <si>
+    <t>Ask</t>
+  </si>
+  <si>
+    <t>Kaufen</t>
+  </si>
+  <si>
+    <t>Bid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="183" formatCode="#,##0.0000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -69,8 +102,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -385,56 +419,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9070A2-3F75-4D79-80D9-D789D642A425}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>54899.31</v>
-      </c>
-      <c r="C2">
-        <v>3.0953999999999999E-2</v>
-      </c>
-      <c r="E2">
-        <v>1699.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>1/A2</f>
+        <v>54899.31</v>
+      </c>
+      <c r="C4">
+        <v>3.0953999999999999E-2</v>
+      </c>
+      <c r="E4">
+        <v>1699.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f>1/A4</f>
         <v>1.8215165181493176E-5</v>
       </c>
-      <c r="C4">
-        <f>A4/C2</f>
+      <c r="C6" s="1">
+        <f>A6/C4</f>
         <v>5.8845917107621553E-4</v>
       </c>
-      <c r="E4">
-        <f>C4*E2</f>
+      <c r="E6" s="1">
+        <f>C6*E4</f>
         <v>1.0000863612440283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>54899.31</v>
+      </c>
+      <c r="C14">
+        <v>3.0953999999999999E-2</v>
+      </c>
+      <c r="E14">
+        <v>1699.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <f>A14/1</f>
+        <v>54899.31</v>
+      </c>
+      <c r="C16" s="1">
+        <f>A16/C14</f>
+        <v>1773577.2436518704</v>
+      </c>
+      <c r="E16" s="1">
+        <f>C16*E14</f>
+        <v>3014194525.5863538</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test calc Arbitrage all 3 Factors
</commit_message>
<xml_diff>
--- a/Calculate.xlsx
+++ b/Calculate.xlsx
@@ -5,36 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixBrenkel\Source\Workspaces\GitHub\cctx-Binance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Workspaces\GitHub\cctx-Binance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6C8D3D-8D00-40D2-951B-34C859967EE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DCCDA1-008E-4851-8ACF-A8BB7A936BBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9030" yWindow="3450" windowWidth="22875" windowHeight="15675" xr2:uid="{40CD4046-9C5B-4F58-A310-3C08BDEFF96F}"/>
+    <workbookView xWindow="4635" yWindow="2580" windowWidth="18600" windowHeight="10260" xr2:uid="{40CD4046-9C5B-4F58-A310-3C08BDEFF96F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>BTC/USDT</t>
   </si>
@@ -71,7 +62,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="183" formatCode="#,##0.0000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -104,7 +95,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -421,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9070A2-3F75-4D79-80D9-D789D642A425}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,10 +492,10 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
         <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -512,10 +503,10 @@
         <v>54899.31</v>
       </c>
       <c r="C14">
+        <v>1699.5</v>
+      </c>
+      <c r="E14">
         <v>3.0953999999999999E-2</v>
-      </c>
-      <c r="E14">
-        <v>1699.5</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -525,20 +516,26 @@
       </c>
       <c r="C16" s="1">
         <f>A16/C14</f>
-        <v>1773577.2436518704</v>
+        <v>32.303212709620475</v>
       </c>
       <c r="E16" s="1">
         <f>C16*E14</f>
-        <v>3014194525.5863538</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>0.99991364621359213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Triples are correctly created
</commit_message>
<xml_diff>
--- a/Calculate.xlsx
+++ b/Calculate.xlsx
@@ -5,27 +5,36 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Workspaces\GitHub\cctx-Binance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixBrenkel\Source\Workspaces\GitHub\cctx-Binance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DCCDA1-008E-4851-8ACF-A8BB7A936BBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E74E8B6-5E39-437D-A6FE-3B309A3110DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="2580" windowWidth="18600" windowHeight="10260" xr2:uid="{40CD4046-9C5B-4F58-A310-3C08BDEFF96F}"/>
+    <workbookView xWindow="11520" yWindow="2250" windowWidth="22875" windowHeight="15675" xr2:uid="{40CD4046-9C5B-4F58-A310-3C08BDEFF96F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>BTC/USDT</t>
   </si>
@@ -55,6 +64,15 @@
   </si>
   <si>
     <t>Bid</t>
+  </si>
+  <si>
+    <t>BNB/BTC</t>
+  </si>
+  <si>
+    <t>SC/BTC</t>
+  </si>
+  <si>
+    <t>SC/BNB</t>
   </si>
 </sst>
 </file>
@@ -410,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9070A2-3F75-4D79-80D9-D789D642A425}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +541,7 @@
         <v>0.99991364621359213</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -531,12 +549,48 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>4.5269999999999998E-3</v>
+      </c>
+      <c r="C24">
+        <v>3.5999999999999999E-7</v>
+      </c>
+      <c r="E24">
+        <v>7.9099999999999998E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f>A24</f>
+        <v>4.5269999999999998E-3</v>
+      </c>
+      <c r="C26">
+        <f>A26/C24</f>
+        <v>12575</v>
+      </c>
+      <c r="E26">
+        <f>C26*E24</f>
+        <v>0.99468250000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>